<commit_message>
added plot for SSites; added to discussion
</commit_message>
<xml_diff>
--- a/thev_transcriptome_ncbi_submission.xlsx
+++ b/thev_transcriptome_ncbi_submission.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abquaye/MyStuff/thev_transcriptome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003BE45D-D958-A549-8F8F-AB3354EE6E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21145299-83F3-544B-A678-DC2583DD277C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="qZzD4R9MHkY34uacjqt3UDyeD61BQpRgIo5GituA+M5TJZYrZGlKZCDSkAkMk0lzHa20F9kBcNHoSPrpZkW+dg==" workbookSaltValue="NTRFdVUfx51db2iwG+fWhA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="13660" yWindow="2920" windowWidth="41120" windowHeight="25720" tabRatio="874" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="41120" windowHeight="25720" tabRatio="874" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="4" r:id="rId1"/>
@@ -2612,7 +2612,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A49" authorId="0" shapeId="0" xr:uid="{6F6EA05E-79A5-4221-8F31-4196F826573E}">
+    <comment ref="A51" authorId="0" shapeId="0" xr:uid="{6F6EA05E-79A5-4221-8F31-4196F826573E}">
       <text>
         <r>
           <rPr>
@@ -2626,7 +2626,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A50" authorId="0" shapeId="0" xr:uid="{4656F1B0-A803-4CE7-B6AD-DD7E0AECE077}">
+    <comment ref="A52" authorId="0" shapeId="0" xr:uid="{4656F1B0-A803-4CE7-B6AD-DD7E0AECE077}">
       <text>
         <r>
           <rPr>
@@ -2640,7 +2640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A51" authorId="0" shapeId="0" xr:uid="{BFA6D1D6-A9C6-487C-93B1-D308A85B2F4C}">
+    <comment ref="A53" authorId="0" shapeId="0" xr:uid="{BFA6D1D6-A9C6-487C-93B1-D308A85B2F4C}">
       <text>
         <r>
           <rPr>
@@ -2664,7 +2664,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A52" authorId="0" shapeId="0" xr:uid="{7DF7F951-E3AA-46C9-9400-4FA052D43573}">
+    <comment ref="A54" authorId="0" shapeId="0" xr:uid="{7DF7F951-E3AA-46C9-9400-4FA052D43573}">
       <text>
         <r>
           <rPr>
@@ -2678,7 +2678,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A53" authorId="0" shapeId="0" xr:uid="{2594ED88-E6B7-439D-A482-5C038E3BCB4A}">
+    <comment ref="A55" authorId="0" shapeId="0" xr:uid="{2594ED88-E6B7-439D-A482-5C038E3BCB4A}">
       <text>
         <r>
           <rPr>
@@ -3011,7 +3011,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A55" authorId="0" shapeId="0" xr:uid="{494BCB97-31DA-4563-A050-36DD8A467D3F}">
+    <comment ref="A57" authorId="0" shapeId="0" xr:uid="{494BCB97-31DA-4563-A050-36DD8A467D3F}">
       <text>
         <r>
           <rPr>
@@ -3103,7 +3103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A56" authorId="0" shapeId="0" xr:uid="{6BCE8D0B-7F45-475A-86B8-E2D963D86E30}">
+    <comment ref="A58" authorId="0" shapeId="0" xr:uid="{6BCE8D0B-7F45-475A-86B8-E2D963D86E30}">
       <text>
         <r>
           <rPr>
@@ -3124,28 +3124,99 @@
         </r>
       </text>
     </comment>
-    <comment ref="A57" authorId="0" shapeId="0" xr:uid="{28C77FE7-DBD7-4513-B8B9-86AC1FA288D3}">
+    <comment ref="A59" authorId="0" shapeId="0" xr:uid="{28C77FE7-DBD7-4513-B8B9-86AC1FA288D3}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Provide details of how processed data files were generated. 
-Steps may include:
-Base-calling software, version, parameters;
-Data filtering steps;
-Read alignment software, version, parameters;
-Additional processing software (e.g., peak-calling, abundance measurement), version, parameters;
-etc.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Steps may include:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Base-calling software, version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Data filtering steps;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Read alignment software, version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Additional processing software (e.g., peak-calling, abundance measurement), version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">etc.
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="A58" authorId="0" shapeId="0" xr:uid="{7621CD5A-1455-9541-849B-2B9271C60879}">
+    <comment ref="A60" authorId="0" shapeId="0" xr:uid="{7621CD5A-1455-9541-849B-2B9271C60879}">
       <text>
         <r>
           <rPr>
@@ -3237,7 +3308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A59" authorId="0" shapeId="0" xr:uid="{F9F4E26C-6F11-4EAE-88A3-FA44B452BC8F}">
+    <comment ref="A61" authorId="0" shapeId="0" xr:uid="{F9F4E26C-6F11-4EAE-88A3-FA44B452BC8F}">
       <text>
         <r>
           <rPr>
@@ -3329,7 +3400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A60" authorId="0" shapeId="0" xr:uid="{5011AF2A-BF87-4698-86BB-C6BE38C846CB}">
+    <comment ref="A62" authorId="0" shapeId="0" xr:uid="{5011AF2A-BF87-4698-86BB-C6BE38C846CB}">
       <text>
         <r>
           <rPr>
@@ -3353,7 +3424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A61" authorId="0" shapeId="0" xr:uid="{5554459D-FEB5-4529-B61F-590DE4D90A1A}">
+    <comment ref="A63" authorId="0" shapeId="0" xr:uid="{5554459D-FEB5-4529-B61F-590DE4D90A1A}">
       <text>
         <r>
           <rPr>
@@ -3367,13 +3438,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="A62" authorId="0" shapeId="0" xr:uid="{68540585-C66C-E44A-A6A1-4FE7B9EEFE45}">
+    <comment ref="A64" authorId="0" shapeId="0" xr:uid="{68540585-C66C-E44A-A6A1-4FE7B9EEFE45}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3381,7 +3452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A63" authorId="0" shapeId="0" xr:uid="{598D1DC7-A9B0-4677-9D1F-2A2B8154AFF5}">
+    <comment ref="A65" authorId="0" shapeId="0" xr:uid="{598D1DC7-A9B0-4677-9D1F-2A2B8154AFF5}">
       <text>
         <r>
           <rPr>
@@ -8316,7 +8387,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="713">
   <si>
     <t>SAMPLES</t>
   </si>
@@ -11256,6 +11327,9 @@
   </si>
   <si>
     <t>c6c7426b7b2b9ea84dee33daec801229</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -12068,17 +12142,8 @@
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="11" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -12095,8 +12160,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="11" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="28">
@@ -16462,10 +16536,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:T80"/>
+  <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView topLeftCell="C12" zoomScale="107" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="107" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="83.6640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -16915,7 +16989,9 @@
       <c r="C36" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="D36" s="14"/>
+      <c r="D36" s="14" t="s">
+        <v>712</v>
+      </c>
       <c r="E36" s="14" t="s">
         <v>618</v>
       </c>
@@ -16962,7 +17038,9 @@
       <c r="C37" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="D37" s="14"/>
+      <c r="D37" s="14" t="s">
+        <v>712</v>
+      </c>
       <c r="E37" s="14" t="s">
         <v>618</v>
       </c>
@@ -17009,7 +17087,9 @@
       <c r="C38" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="D38" s="14"/>
+      <c r="D38" s="14" t="s">
+        <v>712</v>
+      </c>
       <c r="E38" s="14" t="s">
         <v>618</v>
       </c>
@@ -17056,7 +17136,9 @@
       <c r="C39" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="D39" s="14"/>
+      <c r="D39" s="14" t="s">
+        <v>712</v>
+      </c>
       <c r="E39" s="14" t="s">
         <v>618</v>
       </c>
@@ -17105,7 +17187,9 @@
       <c r="C40" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="D40" s="14"/>
+      <c r="D40" s="14" t="s">
+        <v>712</v>
+      </c>
       <c r="E40" s="14" t="s">
         <v>618</v>
       </c>
@@ -17154,7 +17238,9 @@
       <c r="C41" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="D41" s="14"/>
+      <c r="D41" s="14" t="s">
+        <v>712</v>
+      </c>
       <c r="E41" s="14" t="s">
         <v>618</v>
       </c>
@@ -17204,7 +17290,9 @@
       <c r="C42" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="D42" s="14"/>
+      <c r="D42" s="14" t="s">
+        <v>712</v>
+      </c>
       <c r="E42" s="14" t="s">
         <v>618</v>
       </c>
@@ -17254,7 +17342,9 @@
       <c r="C43" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="D43" s="14"/>
+      <c r="D43" s="14" t="s">
+        <v>712</v>
+      </c>
       <c r="E43" s="14" t="s">
         <v>618</v>
       </c>
@@ -17304,7 +17394,9 @@
       <c r="C44" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="D44" s="14"/>
+      <c r="D44" s="14" t="s">
+        <v>712</v>
+      </c>
       <c r="E44" s="14" t="s">
         <v>618</v>
       </c>
@@ -17354,7 +17446,9 @@
       <c r="C45" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="D45" s="14"/>
+      <c r="D45" s="14" t="s">
+        <v>712</v>
+      </c>
       <c r="E45" s="14" t="s">
         <v>618</v>
       </c>
@@ -17444,104 +17538,96 @@
       </c>
       <c r="R46" s="14"/>
     </row>
-    <row r="47" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="9" t="s">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A47" s="37"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A48" s="37"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+    </row>
+    <row r="49" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
-      <c r="J47" s="24"/>
-      <c r="K47" s="24"/>
-      <c r="L47" s="24"/>
-      <c r="M47" s="24"/>
-      <c r="N47" s="24"/>
-      <c r="O47" s="24"/>
-      <c r="P47" s="24"/>
-      <c r="Q47" s="24"/>
-      <c r="R47" s="25"/>
-    </row>
-    <row r="48" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="10" t="s">
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24"/>
+      <c r="K49" s="24"/>
+      <c r="L49" s="24"/>
+      <c r="M49" s="24"/>
+      <c r="N49" s="24"/>
+      <c r="O49" s="24"/>
+      <c r="P49" s="24"/>
+      <c r="Q49" s="24"/>
+      <c r="R49" s="25"/>
+    </row>
+    <row r="50" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
         <v>588</v>
       </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="10"/>
-      <c r="M48" s="10"/>
-      <c r="N48" s="10"/>
-      <c r="O48" s="10"/>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="10"/>
-      <c r="R48" s="11"/>
-    </row>
-    <row r="49" spans="1:18" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="13" t="s">
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="11"/>
+    </row>
+    <row r="51" spans="1:18" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="B49" s="43" t="s">
+      <c r="B51" s="43" t="s">
         <v>649</v>
-      </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-    </row>
-    <row r="50" spans="1:18" ht="78" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="B50" s="43" t="s">
-        <v>650</v>
-      </c>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
-      <c r="P50" s="14"/>
-      <c r="Q50" s="14"/>
-      <c r="R50" s="14"/>
-    </row>
-    <row r="51" spans="1:18" ht="28" x14ac:dyDescent="0.2">
-      <c r="A51" s="13" t="s">
-        <v>362</v>
-      </c>
-      <c r="B51" s="43" t="s">
-        <v>648</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
@@ -17560,12 +17646,12 @@
       <c r="Q51" s="14"/>
       <c r="R51" s="14"/>
     </row>
-    <row r="52" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:18" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="B52" s="72" t="s">
-        <v>651</v>
+        <v>361</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>650</v>
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
@@ -17584,12 +17670,12 @@
       <c r="Q52" s="14"/>
       <c r="R52" s="14"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" ht="28" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>647</v>
+        <v>362</v>
+      </c>
+      <c r="B53" s="43" t="s">
+        <v>648</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
@@ -17608,9 +17694,13 @@
       <c r="Q53" s="14"/>
       <c r="R53" s="14"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A54" s="13"/>
-      <c r="B54" s="14"/>
+    <row r="54" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+      <c r="A54" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="B54" s="72" t="s">
+        <v>651</v>
+      </c>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
@@ -17630,10 +17720,10 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>669</v>
+        <v>647</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
@@ -17652,13 +17742,9 @@
       <c r="Q55" s="14"/>
       <c r="R55" s="14"/>
     </row>
-    <row r="56" spans="1:18" ht="42" x14ac:dyDescent="0.2">
-      <c r="A56" s="13" t="s">
-        <v>565</v>
-      </c>
-      <c r="B56" s="43" t="s">
-        <v>670</v>
-      </c>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A56" s="13"/>
+      <c r="B56" s="14"/>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
@@ -17676,12 +17762,12 @@
       <c r="Q56" s="14"/>
       <c r="R56" s="14"/>
     </row>
-    <row r="57" spans="1:18" ht="42" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
-        <v>565</v>
-      </c>
-      <c r="B57" s="43" t="s">
-        <v>671</v>
+        <v>364</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>669</v>
       </c>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
@@ -17705,7 +17791,7 @@
         <v>565</v>
       </c>
       <c r="B58" s="43" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
@@ -17724,12 +17810,12 @@
       <c r="Q58" s="14"/>
       <c r="R58" s="14"/>
     </row>
-    <row r="59" spans="1:18" ht="28" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
         <v>565</v>
       </c>
       <c r="B59" s="43" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
@@ -17748,12 +17834,12 @@
       <c r="Q59" s="14"/>
       <c r="R59" s="14"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>652</v>
+        <v>565</v>
+      </c>
+      <c r="B60" s="43" t="s">
+        <v>672</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
@@ -17772,12 +17858,12 @@
       <c r="Q60" s="14"/>
       <c r="R60" s="14"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" ht="28" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="B61" s="14" t="s">
-        <v>674</v>
+        <v>565</v>
+      </c>
+      <c r="B61" s="43" t="s">
+        <v>673</v>
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
@@ -17798,10 +17884,10 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">
-        <v>582</v>
+        <v>365</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>675</v>
+        <v>652</v>
       </c>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
@@ -17822,10 +17908,10 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
-        <v>582</v>
+        <v>366</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
@@ -17845,94 +17931,98 @@
       <c r="R63" s="14"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A64" s="27"/>
-      <c r="B64" s="27"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="27"/>
-      <c r="I64" s="27"/>
-      <c r="J64" s="27"/>
-      <c r="K64" s="27"/>
-      <c r="L64" s="27"/>
-      <c r="M64" s="27"/>
-      <c r="N64" s="27"/>
-      <c r="O64" s="27"/>
-      <c r="P64" s="27"/>
-      <c r="Q64" s="27"/>
-      <c r="R64" s="27"/>
-    </row>
-    <row r="65" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="9" t="s">
+      <c r="A64" s="13" t="s">
+        <v>582</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>675</v>
+      </c>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="14"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="14"/>
+      <c r="P64" s="14"/>
+      <c r="Q64" s="14"/>
+      <c r="R64" s="14"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A65" s="13" t="s">
+        <v>582</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>676</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
+      <c r="N65" s="14"/>
+      <c r="O65" s="14"/>
+      <c r="P65" s="14"/>
+      <c r="Q65" s="14"/>
+      <c r="R65" s="14"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A66" s="27"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="27"/>
+      <c r="H66" s="27"/>
+      <c r="I66" s="27"/>
+      <c r="J66" s="27"/>
+      <c r="K66" s="27"/>
+      <c r="L66" s="27"/>
+      <c r="M66" s="27"/>
+      <c r="N66" s="27"/>
+      <c r="O66" s="27"/>
+      <c r="P66" s="27"/>
+      <c r="Q66" s="27"/>
+      <c r="R66" s="27"/>
+    </row>
+    <row r="67" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="24"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="24"/>
-      <c r="H65" s="24"/>
-      <c r="I65" s="24"/>
-      <c r="J65" s="24"/>
-      <c r="K65" s="24"/>
-      <c r="L65" s="24"/>
-      <c r="M65" s="24"/>
-      <c r="N65" s="24"/>
-      <c r="O65" s="24"/>
-      <c r="P65" s="24"/>
-      <c r="Q65" s="24"/>
-      <c r="R65" s="25"/>
-    </row>
-    <row r="66" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="10"/>
-      <c r="H66" s="10"/>
-      <c r="I66" s="10"/>
-      <c r="J66" s="10"/>
-      <c r="K66" s="10"/>
-      <c r="L66" s="10"/>
-      <c r="M66" s="10"/>
-      <c r="N66" s="10"/>
-      <c r="O66" s="10"/>
-      <c r="P66" s="10"/>
-      <c r="Q66" s="10"/>
-      <c r="R66" s="11"/>
-    </row>
-    <row r="67" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
-      <c r="H67" s="10"/>
-      <c r="I67" s="10"/>
-      <c r="J67" s="10"/>
-      <c r="K67" s="10"/>
-      <c r="L67" s="10"/>
-      <c r="M67" s="10"/>
-      <c r="N67" s="10"/>
-      <c r="O67" s="10"/>
-      <c r="P67" s="10"/>
-      <c r="Q67" s="10"/>
-      <c r="R67" s="11"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="24"/>
+      <c r="I67" s="24"/>
+      <c r="J67" s="24"/>
+      <c r="K67" s="24"/>
+      <c r="L67" s="24"/>
+      <c r="M67" s="24"/>
+      <c r="N67" s="24"/>
+      <c r="O67" s="24"/>
+      <c r="P67" s="24"/>
+      <c r="Q67" s="24"/>
+      <c r="R67" s="25"/>
     </row>
     <row r="68" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -17952,142 +18042,186 @@
       <c r="Q68" s="10"/>
       <c r="R68" s="11"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A69" s="55" t="s">
+    <row r="69" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
+      <c r="N69" s="10"/>
+      <c r="O69" s="10"/>
+      <c r="P69" s="10"/>
+      <c r="Q69" s="10"/>
+      <c r="R69" s="11"/>
+    </row>
+    <row r="70" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="10"/>
+      <c r="K70" s="10"/>
+      <c r="L70" s="10"/>
+      <c r="M70" s="10"/>
+      <c r="N70" s="10"/>
+      <c r="O70" s="10"/>
+      <c r="P70" s="10"/>
+      <c r="Q70" s="10"/>
+      <c r="R70" s="11"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A71" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="55" t="s">
+      <c r="B71" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="55"/>
-      <c r="D69" s="55"/>
-      <c r="E69" s="55"/>
-      <c r="F69" s="55"/>
-      <c r="G69" s="55"/>
-      <c r="H69" s="55"/>
-      <c r="I69" s="55"/>
-      <c r="J69" s="55"/>
-      <c r="K69" s="55"/>
-      <c r="L69" s="55"/>
-      <c r="M69" s="55"/>
-      <c r="N69" s="55"/>
-      <c r="O69" s="55"/>
-      <c r="P69" s="55"/>
-      <c r="Q69" s="55"/>
-      <c r="R69" s="55"/>
-      <c r="S69" s="56"/>
-      <c r="T69" s="56"/>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A70" s="14" t="s">
+      <c r="C71" s="55"/>
+      <c r="D71" s="55"/>
+      <c r="E71" s="55"/>
+      <c r="F71" s="55"/>
+      <c r="G71" s="55"/>
+      <c r="H71" s="55"/>
+      <c r="I71" s="55"/>
+      <c r="J71" s="55"/>
+      <c r="K71" s="55"/>
+      <c r="L71" s="55"/>
+      <c r="M71" s="55"/>
+      <c r="N71" s="55"/>
+      <c r="O71" s="55"/>
+      <c r="P71" s="55"/>
+      <c r="Q71" s="55"/>
+      <c r="R71" s="55"/>
+      <c r="S71" s="56"/>
+      <c r="T71" s="56"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A72" s="14" t="s">
         <v>624</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B72" s="14" t="s">
         <v>623</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A71" s="14" t="s">
-        <v>625</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A72" s="8" t="s">
-        <v>627</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73" s="14" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A74" s="14" t="s">
-        <v>631</v>
+      <c r="A74" s="8" t="s">
+        <v>627</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75" s="14" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" s="14" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77" s="14" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78" s="14" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" s="14" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
+        <v>639</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="14" t="s">
+        <v>641</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="14" t="s">
         <v>643</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B82" s="14" t="s">
         <v>644</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0"/>
   <phoneticPr fontId="34" type="noConversion"/>
-  <conditionalFormatting sqref="A36:A46">
+  <conditionalFormatting sqref="A36:A48">
     <cfRule type="duplicateValues" dxfId="12" priority="493"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A73:B74 A70:B71 B72">
+  <conditionalFormatting sqref="A75:B76 A72:B73 B74">
     <cfRule type="duplicateValues" dxfId="11" priority="496"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A81:M1048576 C70:M80 N70:XFD1048576">
+  <conditionalFormatting sqref="A83:M1048576 C72:M82 N72:XFD1048576">
     <cfRule type="duplicateValues" dxfId="10" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36:B46">
+  <conditionalFormatting sqref="B36:B48">
     <cfRule type="duplicateValues" dxfId="9" priority="495"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C28">
     <cfRule type="duplicateValues" dxfId="8" priority="27"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C63">
+  <conditionalFormatting sqref="C51:C65">
     <cfRule type="duplicateValues" dxfId="7" priority="501"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R41:XFD46 P36:XFD37 P39:XFD40 Q38:XFD38">
+  <conditionalFormatting sqref="R41:XFD48 P36:XFD37 P39:XFD40 Q38:XFD38">
     <cfRule type="duplicateValues" dxfId="6" priority="470"/>
   </conditionalFormatting>
   <dataValidations xWindow="367" yWindow="405" count="17">
@@ -18102,22 +18236,22 @@
       <formula1>50</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="List the name of any processed data files (one per row) that were derived from multiple samples. For instance, bulkRNA-seq tables that include library names as headers, or &quot;merged&quot; peak files." sqref="B20:C20" xr:uid="{38E8CDD9-437B-46E7-BC82-569009D0AD05}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the treatment(s) applied to the sample. If no treatments were applied enter 'none'. _x000a_**NOTE: You can insert additional columns before 'molecule' and add more sample descriptions - clinical data, for example**_x000a_" sqref="H36:H46" xr:uid="{DD3BF453-67A7-457F-8A50-2AA2F9C643F5}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C53 B20" xr:uid="{1DA8B795-5C89-4577-8836-DB7AEFB725B7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specify the library strategy. For example: RNA-seq, scRNA-seq, CITE-seq, Spatial Transcriptomics, ChIP-Seq, CUT&amp;Tag, Bisulfite-seq, ATAC-seq, Hi-C, and so on..." sqref="B53" xr:uid="{3E1B337C-0FAB-46AD-AF75-6E2448C62637}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Identify the organism(s) from which the sequences were derived.  For example:_x000a_Homo sapiens_x000a_Mus musculus_x000a_Arabidopsis thaliana_x000a_Escherichia coli K-12_x000a_Caenorhabditis elegans" sqref="C46:D46 D41:D45 C36:C45" xr:uid="{A870C9A2-F05A-485A-9E21-08C3F86683B5}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the treatment(s) applied to the sample. If no treatments were applied enter 'none'. _x000a_**NOTE: You can insert additional columns before 'molecule' and add more sample descriptions - clinical data, for example**_x000a_" sqref="H36:H48" xr:uid="{DD3BF453-67A7-457F-8A50-2AA2F9C643F5}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C55 B20" xr:uid="{1DA8B795-5C89-4577-8836-DB7AEFB725B7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specify the library strategy. For example: RNA-seq, scRNA-seq, CITE-seq, Spatial Transcriptomics, ChIP-Seq, CUT&amp;Tag, Bisulfite-seq, ATAC-seq, Hi-C, and so on..." sqref="B55" xr:uid="{3E1B337C-0FAB-46AD-AF75-6E2448C62637}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Identify the organism(s) from which the sequences were derived.  For example:_x000a_Homo sapiens_x000a_Mus musculus_x000a_Arabidopsis thaliana_x000a_Escherichia coli K-12_x000a_Caenorhabditis elegans" sqref="C46:D48 D41:D45 C36:C45" xr:uid="{A870C9A2-F05A-485A-9E21-08C3F86683B5}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the tissue from which this sample was derived. For example:_x000a_Liver_x000a_Breast cancer_x000a_Colorectal cancer_x000a_Liver tumor_x000a_Whole organism_x000a_Mycelium" sqref="D36:D40" xr:uid="{F363101B-E3EB-4921-89A5-DE79B20B09EF}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Treatment(s) applied to the sample. If no treatments were applied enter 'none'. _x000a_**NOTE: You can insert additional columns before 'molecule' and add more sample descriptions - clinical data, for example**_x000a_" sqref="H37:H46" xr:uid="{47B6B633-8A68-4530-9AD8-BD49CE875996}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the drop down menu" sqref="I36:I46" xr:uid="{4B61C4DA-D826-4533-9531-93FAAFEF6886}">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Treatment(s) applied to the sample. If no treatments were applied enter 'none'. _x000a_**NOTE: You can insert additional columns before 'molecule' and add more sample descriptions - clinical data, for example**_x000a_" sqref="H37:H48" xr:uid="{47B6B633-8A68-4530-9AD8-BD49CE875996}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the drop down menu" sqref="I36:I48" xr:uid="{4B61C4DA-D826-4533-9531-93FAAFEF6886}">
       <formula1>"polyA RNA,total RNA, nuclear RNA, cytoplasmic RNA, genomic DNA,protein,other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the drop down menu" sqref="J36:J46" xr:uid="{4DF3746A-E025-4F6A-B7CC-339891AC2027}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the drop down menu" sqref="J36:J48" xr:uid="{4DF3746A-E025-4F6A-B7CC-339891AC2027}">
       <formula1>"single,paired-end"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the cell line used, if applicable. For example:_x000a_HeLa_x000a_HEK293_x000a_A549" sqref="E36:E46" xr:uid="{22185DB1-F1B6-4642-9A12-2889E7D560EC}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the cell type. Examples include:_x000a_PBMCs_x000a_Adipocytes_x000a_neural progenitor cells (NPCs)_x000a_" sqref="F36:F46" xr:uid="{AD947475-09CC-48B9-8265-B9811301F615}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the genotype (if applicable). If not applicable change &quot;genotype&quot; to something else. For example: strain, sex, cultivar, breed, age, developmental stage, etc" sqref="G36:G46" xr:uid="{E4E9BB68-E9AC-40EB-9161-0960CBF212EC}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Each sample title should be unique. _x000a_Use biol/tech rep numbers (when _x000a_applicable) to unique the titles. _x000a_For example:_x000a_Muscle, exercised, 60min, biol rep1_x000a_Muscle, exercised, 60min, biol rep2_x000a_" sqref="B36:C46" xr:uid="{16FCC838-0E0E-48E4-B2AA-D96D65E76279}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the cell line used, if applicable. For example:_x000a_HeLa_x000a_HEK293_x000a_A549" sqref="E36:E48" xr:uid="{22185DB1-F1B6-4642-9A12-2889E7D560EC}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the cell type. Examples include:_x000a_PBMCs_x000a_Adipocytes_x000a_neural progenitor cells (NPCs)_x000a_" sqref="F36:F48" xr:uid="{AD947475-09CC-48B9-8265-B9811301F615}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the genotype (if applicable). If not applicable change &quot;genotype&quot; to something else. For example: strain, sex, cultivar, breed, age, developmental stage, etc" sqref="G36:G48" xr:uid="{E4E9BB68-E9AC-40EB-9161-0960CBF212EC}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Each sample title should be unique. _x000a_Use biol/tech rep numbers (when _x000a_applicable) to unique the titles. _x000a_For example:_x000a_Muscle, exercised, 60min, biol rep1_x000a_Muscle, exercised, 60min, biol rep2_x000a_" sqref="B36:C48" xr:uid="{16FCC838-0E0E-48E4-B2AA-D96D65E76279}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18130,7 +18264,7 @@
           <x14:formula1>
             <xm:f>'Data validation'!$A$2:$A$58</xm:f>
           </x14:formula1>
-          <xm:sqref>K46:L46 L41:L45 K36:K45</xm:sqref>
+          <xm:sqref>K46:L48 L41:L45 K36:K45</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -18145,7 +18279,7 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -18157,32 +18291,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="74" t="s">
         <v>589</v>
       </c>
-      <c r="B1" s="77"/>
+      <c r="B1" s="74"/>
     </row>
     <row r="2" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="81" t="s">
         <v>594</v>
       </c>
-      <c r="B2" s="75"/>
+      <c r="B2" s="81"/>
     </row>
     <row r="3" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="76"/>
+      <c r="B3" s="82"/>
     </row>
     <row r="4" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="79" t="s">
         <v>595</v>
       </c>
-      <c r="B4" s="73"/>
+      <c r="B4" s="79"/>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="81"/>
-      <c r="B5" s="81"/>
+      <c r="A5" s="78"/>
+      <c r="B5" s="78"/>
     </row>
     <row r="6" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -18279,80 +18413,80 @@
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="73"/>
-      <c r="B17" s="73"/>
+      <c r="A17" s="79"/>
+      <c r="B17" s="79"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="75" t="s">
         <v>266</v>
       </c>
-      <c r="B18" s="79"/>
+      <c r="B18" s="76"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="77" t="s">
         <v>563</v>
       </c>
-      <c r="B19" s="80"/>
+      <c r="B19" s="77"/>
     </row>
     <row r="20" spans="1:6" ht="136.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="80" t="s">
         <v>591</v>
       </c>
-      <c r="B20" s="74"/>
+      <c r="B20" s="80"/>
       <c r="F20" s="63"/>
     </row>
     <row r="21" spans="1:6" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="80" t="s">
         <v>592</v>
       </c>
-      <c r="B21" s="74"/>
+      <c r="B21" s="80"/>
     </row>
     <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
+      <c r="A22" s="79"/>
+      <c r="B22" s="79"/>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="73"/>
-      <c r="B24" s="73"/>
+      <c r="A24" s="79"/>
+      <c r="B24" s="79"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="73"/>
-      <c r="B25" s="73"/>
+      <c r="A25" s="79"/>
+      <c r="B25" s="79"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="73"/>
-      <c r="B26" s="73"/>
+      <c r="A26" s="79"/>
+      <c r="B26" s="79"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="73"/>
-      <c r="B27" s="73"/>
+      <c r="A27" s="79"/>
+      <c r="B27" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" location="categories" xr:uid="{D6250736-B96D-4C3E-A39D-F5873CF8B173}"/>
@@ -18380,7 +18514,7 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -18476,7 +18610,7 @@
       <c r="F11" s="14" t="s">
         <v>658</v>
       </c>
-      <c r="G11" s="82" t="s">
+      <c r="G11" s="73" t="s">
         <v>701</v>
       </c>
     </row>
@@ -18656,7 +18790,7 @@
       <c r="A26" s="14" t="s">
         <v>636</v>
       </c>
-      <c r="B26" s="82" t="s">
+      <c r="B26" s="73" t="s">
         <v>690</v>
       </c>
     </row>
@@ -18693,14 +18827,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A31:G1048576 B22:G30 B9:E21 G9:G21">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A12:A13 A9:A10">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:A24">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:G1048576 B22:G30 B9:E21 G9:G21">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18712,7 +18846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B97CE2-DFAA-450B-948E-0D22EC57AEF0}">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -25649,13 +25783,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="uHeIq0fTY+SkfiG0BUBfkRWN7VsHdDGQfAJwovwYuwp6zuFwWIwuY7JnUgHrIwBV4G25XMH5B7S3rMfU5U3akw==" saltValue="Zz3TVxIHK82bnZabgvGk9Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <conditionalFormatting sqref="A61:E69">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:Y31">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T26:Y31">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the drop down menu" sqref="I30:K32" xr:uid="{79D6ECAE-44AD-41AB-84C9-88F44BE0AE81}">

</xml_diff>